<commit_message>
new function to deal with data on one csv file
</commit_message>
<xml_diff>
--- a/user_input_data/input_template.xlsx
+++ b/user_input_data/input_template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t xml:space="preserve">ES</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ohio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">watershed</t>
   </si>
   <si>
     <t xml:space="preserve">ethonal production</t>
@@ -190,8 +187,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,193 +216,193 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>3200</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>6400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>50000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <f aca="false">1/K4</f>
         <v>2E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>2000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>10050001</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>900</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>2000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>5200</v>
       </c>
     </row>
@@ -424,196 +425,196 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>5500</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>60000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <f aca="false">1/K4</f>
         <v>1.66666666666667E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>2700</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>520</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>4100002</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>1040</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>1200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>3950</v>
       </c>
     </row>
@@ -636,196 +637,196 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>4200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>80000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <f aca="false">1/K4</f>
         <v>1.25E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>3900</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>10050001</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>907</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>2088</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>3200</v>
       </c>
     </row>

</xml_diff>